<commit_message>
Linhas de intervalo e checksboxs
</commit_message>
<xml_diff>
--- a/dados_exemplo/teste_sem_ultima.xlsx
+++ b/dados_exemplo/teste_sem_ultima.xlsx
@@ -130,11 +130,11 @@
   </sheetPr>
   <dimension ref="A1:CS240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CA211" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CU233" activeCellId="0" sqref="CU233"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CU11" activeCellId="0" sqref="CU11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.33"/>
   </cols>
@@ -422,15 +422,9 @@
       <c r="CP1" s="2" t="n">
         <v>0.082</v>
       </c>
-      <c r="CQ1" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR1" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS1" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ1" s="2"/>
+      <c r="CR1" s="2"/>
+      <c r="CS1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -715,15 +709,9 @@
       <c r="CP2" s="2" t="n">
         <v>0.083</v>
       </c>
-      <c r="CQ2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS2" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ2" s="2"/>
+      <c r="CR2" s="2"/>
+      <c r="CS2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -1008,15 +996,9 @@
       <c r="CP3" s="2" t="n">
         <v>0.089</v>
       </c>
-      <c r="CQ3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS3" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ3" s="2"/>
+      <c r="CR3" s="2"/>
+      <c r="CS3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -1301,15 +1283,9 @@
       <c r="CP4" s="2" t="n">
         <v>0.094</v>
       </c>
-      <c r="CQ4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS4" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ4" s="2"/>
+      <c r="CR4" s="2"/>
+      <c r="CS4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -1594,15 +1570,9 @@
       <c r="CP5" s="2" t="n">
         <v>0.096</v>
       </c>
-      <c r="CQ5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS5" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ5" s="2"/>
+      <c r="CR5" s="2"/>
+      <c r="CS5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -1887,15 +1857,9 @@
       <c r="CP6" s="2" t="n">
         <v>0.101</v>
       </c>
-      <c r="CQ6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS6" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ6" s="2"/>
+      <c r="CR6" s="2"/>
+      <c r="CS6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -2180,15 +2144,9 @@
       <c r="CP7" s="2" t="n">
         <v>0.107</v>
       </c>
-      <c r="CQ7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS7" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ7" s="2"/>
+      <c r="CR7" s="2"/>
+      <c r="CS7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -2473,15 +2431,9 @@
       <c r="CP8" s="2" t="n">
         <v>0.111</v>
       </c>
-      <c r="CQ8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS8" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ8" s="2"/>
+      <c r="CR8" s="2"/>
+      <c r="CS8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -2766,15 +2718,9 @@
       <c r="CP9" s="2" t="n">
         <v>0.114</v>
       </c>
-      <c r="CQ9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS9" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ9" s="2"/>
+      <c r="CR9" s="2"/>
+      <c r="CS9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -3059,15 +3005,9 @@
       <c r="CP10" s="2" t="n">
         <v>0.122</v>
       </c>
-      <c r="CQ10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS10" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ10" s="2"/>
+      <c r="CR10" s="2"/>
+      <c r="CS10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -3352,15 +3292,9 @@
       <c r="CP11" s="2" t="n">
         <v>0.125</v>
       </c>
-      <c r="CQ11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS11" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ11" s="2"/>
+      <c r="CR11" s="2"/>
+      <c r="CS11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -3645,15 +3579,9 @@
       <c r="CP12" s="2" t="n">
         <v>0.132</v>
       </c>
-      <c r="CQ12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS12" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ12" s="2"/>
+      <c r="CR12" s="2"/>
+      <c r="CS12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -3938,15 +3866,9 @@
       <c r="CP13" s="2" t="n">
         <v>0.139</v>
       </c>
-      <c r="CQ13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS13" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ13" s="2"/>
+      <c r="CR13" s="2"/>
+      <c r="CS13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -4231,15 +4153,9 @@
       <c r="CP14" s="2" t="n">
         <v>0.146</v>
       </c>
-      <c r="CQ14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS14" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ14" s="2"/>
+      <c r="CR14" s="2"/>
+      <c r="CS14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -4524,15 +4440,9 @@
       <c r="CP15" s="2" t="n">
         <v>0.155</v>
       </c>
-      <c r="CQ15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS15" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ15" s="2"/>
+      <c r="CR15" s="2"/>
+      <c r="CS15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -4817,15 +4727,9 @@
       <c r="CP16" s="2" t="n">
         <v>0.163</v>
       </c>
-      <c r="CQ16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS16" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ16" s="2"/>
+      <c r="CR16" s="2"/>
+      <c r="CS16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -5110,15 +5014,9 @@
       <c r="CP17" s="2" t="n">
         <v>0.169</v>
       </c>
-      <c r="CQ17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS17" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ17" s="2"/>
+      <c r="CR17" s="2"/>
+      <c r="CS17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -5403,15 +5301,9 @@
       <c r="CP18" s="2" t="n">
         <v>0.18</v>
       </c>
-      <c r="CQ18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS18" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ18" s="2"/>
+      <c r="CR18" s="2"/>
+      <c r="CS18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -5696,15 +5588,9 @@
       <c r="CP19" s="2" t="n">
         <v>0.191</v>
       </c>
-      <c r="CQ19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS19" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ19" s="2"/>
+      <c r="CR19" s="2"/>
+      <c r="CS19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -5989,15 +5875,9 @@
       <c r="CP20" s="2" t="n">
         <v>0.203</v>
       </c>
-      <c r="CQ20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS20" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ20" s="2"/>
+      <c r="CR20" s="2"/>
+      <c r="CS20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -6282,15 +6162,9 @@
       <c r="CP21" s="2" t="n">
         <v>0.214</v>
       </c>
-      <c r="CQ21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS21" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ21" s="2"/>
+      <c r="CR21" s="2"/>
+      <c r="CS21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -6575,15 +6449,9 @@
       <c r="CP22" s="2" t="n">
         <v>0.225</v>
       </c>
-      <c r="CQ22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS22" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ22" s="2"/>
+      <c r="CR22" s="2"/>
+      <c r="CS22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -6868,15 +6736,9 @@
       <c r="CP23" s="2" t="n">
         <v>0.239</v>
       </c>
-      <c r="CQ23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS23" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ23" s="2"/>
+      <c r="CR23" s="2"/>
+      <c r="CS23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -7161,15 +7023,9 @@
       <c r="CP24" s="2" t="n">
         <v>0.251</v>
       </c>
-      <c r="CQ24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS24" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ24" s="2"/>
+      <c r="CR24" s="2"/>
+      <c r="CS24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -7454,15 +7310,9 @@
       <c r="CP25" s="2" t="n">
         <v>0.268</v>
       </c>
-      <c r="CQ25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS25" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ25" s="2"/>
+      <c r="CR25" s="2"/>
+      <c r="CS25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -7747,15 +7597,9 @@
       <c r="CP26" s="2" t="n">
         <v>0.279</v>
       </c>
-      <c r="CQ26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS26" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ26" s="2"/>
+      <c r="CR26" s="2"/>
+      <c r="CS26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -8040,15 +7884,9 @@
       <c r="CP27" s="2" t="n">
         <v>0.295</v>
       </c>
-      <c r="CQ27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS27" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ27" s="2"/>
+      <c r="CR27" s="2"/>
+      <c r="CS27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -8333,15 +8171,9 @@
       <c r="CP28" s="2" t="n">
         <v>0.311</v>
       </c>
-      <c r="CQ28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS28" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ28" s="2"/>
+      <c r="CR28" s="2"/>
+      <c r="CS28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -8626,15 +8458,9 @@
       <c r="CP29" s="2" t="n">
         <v>0.326</v>
       </c>
-      <c r="CQ29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS29" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ29" s="2"/>
+      <c r="CR29" s="2"/>
+      <c r="CS29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
@@ -8919,15 +8745,9 @@
       <c r="CP30" s="2" t="n">
         <v>0.343</v>
       </c>
-      <c r="CQ30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS30" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ30" s="2"/>
+      <c r="CR30" s="2"/>
+      <c r="CS30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
@@ -9212,15 +9032,9 @@
       <c r="CP31" s="2" t="n">
         <v>0.356</v>
       </c>
-      <c r="CQ31" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR31" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS31" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ31" s="2"/>
+      <c r="CR31" s="2"/>
+      <c r="CS31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
@@ -9505,15 +9319,9 @@
       <c r="CP32" s="2" t="n">
         <v>0.372</v>
       </c>
-      <c r="CQ32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS32" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ32" s="2"/>
+      <c r="CR32" s="2"/>
+      <c r="CS32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
@@ -9798,15 +9606,9 @@
       <c r="CP33" s="2" t="n">
         <v>0.385</v>
       </c>
-      <c r="CQ33" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR33" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS33" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ33" s="2"/>
+      <c r="CR33" s="2"/>
+      <c r="CS33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
@@ -10091,15 +9893,9 @@
       <c r="CP34" s="2" t="n">
         <v>0.403</v>
       </c>
-      <c r="CQ34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS34" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ34" s="2"/>
+      <c r="CR34" s="2"/>
+      <c r="CS34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -10384,15 +10180,9 @@
       <c r="CP35" s="2" t="n">
         <v>0.419</v>
       </c>
-      <c r="CQ35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS35" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ35" s="2"/>
+      <c r="CR35" s="2"/>
+      <c r="CS35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -10677,15 +10467,9 @@
       <c r="CP36" s="2" t="n">
         <v>0.434</v>
       </c>
-      <c r="CQ36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS36" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ36" s="2"/>
+      <c r="CR36" s="2"/>
+      <c r="CS36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -10970,15 +10754,9 @@
       <c r="CP37" s="2" t="n">
         <v>0.453</v>
       </c>
-      <c r="CQ37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS37" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ37" s="2"/>
+      <c r="CR37" s="2"/>
+      <c r="CS37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -11263,15 +11041,9 @@
       <c r="CP38" s="2" t="n">
         <v>0.469</v>
       </c>
-      <c r="CQ38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS38" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ38" s="2"/>
+      <c r="CR38" s="2"/>
+      <c r="CS38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
@@ -11556,15 +11328,9 @@
       <c r="CP39" s="2" t="n">
         <v>0.479</v>
       </c>
-      <c r="CQ39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS39" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ39" s="2"/>
+      <c r="CR39" s="2"/>
+      <c r="CS39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
@@ -11849,15 +11615,9 @@
       <c r="CP40" s="2" t="n">
         <v>0.501</v>
       </c>
-      <c r="CQ40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS40" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ40" s="2"/>
+      <c r="CR40" s="2"/>
+      <c r="CS40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
@@ -12142,15 +11902,9 @@
       <c r="CP41" s="2" t="n">
         <v>0.521</v>
       </c>
-      <c r="CQ41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS41" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ41" s="2"/>
+      <c r="CR41" s="2"/>
+      <c r="CS41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
@@ -12435,15 +12189,9 @@
       <c r="CP42" s="2" t="n">
         <v>0.533</v>
       </c>
-      <c r="CQ42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS42" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ42" s="2"/>
+      <c r="CR42" s="2"/>
+      <c r="CS42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
@@ -12728,15 +12476,9 @@
       <c r="CP43" s="2" t="n">
         <v>0.553</v>
       </c>
-      <c r="CQ43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS43" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ43" s="2"/>
+      <c r="CR43" s="2"/>
+      <c r="CS43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
@@ -13021,15 +12763,9 @@
       <c r="CP44" s="2" t="n">
         <v>0.57</v>
       </c>
-      <c r="CQ44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS44" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ44" s="2"/>
+      <c r="CR44" s="2"/>
+      <c r="CS44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -13314,15 +13050,9 @@
       <c r="CP45" s="2" t="n">
         <v>0.589</v>
       </c>
-      <c r="CQ45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS45" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ45" s="2"/>
+      <c r="CR45" s="2"/>
+      <c r="CS45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
@@ -13607,15 +13337,9 @@
       <c r="CP46" s="2" t="n">
         <v>0.606</v>
       </c>
-      <c r="CQ46" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR46" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS46" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ46" s="2"/>
+      <c r="CR46" s="2"/>
+      <c r="CS46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -13900,15 +13624,9 @@
       <c r="CP47" s="2" t="n">
         <v>0.623</v>
       </c>
-      <c r="CQ47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS47" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ47" s="2"/>
+      <c r="CR47" s="2"/>
+      <c r="CS47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
@@ -14193,15 +13911,9 @@
       <c r="CP48" s="2" t="n">
         <v>0.638</v>
       </c>
-      <c r="CQ48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS48" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ48" s="2"/>
+      <c r="CR48" s="2"/>
+      <c r="CS48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
@@ -14486,15 +14198,9 @@
       <c r="CP49" s="2" t="n">
         <v>0.663</v>
       </c>
-      <c r="CQ49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS49" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ49" s="2"/>
+      <c r="CR49" s="2"/>
+      <c r="CS49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
@@ -14779,15 +14485,9 @@
       <c r="CP50" s="2" t="n">
         <v>0.676</v>
       </c>
-      <c r="CQ50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS50" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ50" s="2"/>
+      <c r="CR50" s="2"/>
+      <c r="CS50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
@@ -15072,15 +14772,9 @@
       <c r="CP51" s="2" t="n">
         <v>0.691</v>
       </c>
-      <c r="CQ51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS51" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ51" s="2"/>
+      <c r="CR51" s="2"/>
+      <c r="CS51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
@@ -15365,15 +15059,9 @@
       <c r="CP52" s="2" t="n">
         <v>0.711</v>
       </c>
-      <c r="CQ52" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR52" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS52" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ52" s="2"/>
+      <c r="CR52" s="2"/>
+      <c r="CS52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
@@ -15658,15 +15346,9 @@
       <c r="CP53" s="2" t="n">
         <v>0.73</v>
       </c>
-      <c r="CQ53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS53" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ53" s="2"/>
+      <c r="CR53" s="2"/>
+      <c r="CS53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
@@ -15951,15 +15633,9 @@
       <c r="CP54" s="2" t="n">
         <v>0.749</v>
       </c>
-      <c r="CQ54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS54" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ54" s="2"/>
+      <c r="CR54" s="2"/>
+      <c r="CS54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
@@ -16244,15 +15920,9 @@
       <c r="CP55" s="2" t="n">
         <v>0.771</v>
       </c>
-      <c r="CQ55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS55" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ55" s="2"/>
+      <c r="CR55" s="2"/>
+      <c r="CS55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
@@ -16537,15 +16207,9 @@
       <c r="CP56" s="2" t="n">
         <v>0.78</v>
       </c>
-      <c r="CQ56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS56" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ56" s="2"/>
+      <c r="CR56" s="2"/>
+      <c r="CS56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
@@ -16830,15 +16494,9 @@
       <c r="CP57" s="2" t="n">
         <v>0.807</v>
       </c>
-      <c r="CQ57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS57" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ57" s="2"/>
+      <c r="CR57" s="2"/>
+      <c r="CS57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
@@ -17123,15 +16781,9 @@
       <c r="CP58" s="2" t="n">
         <v>0.83</v>
       </c>
-      <c r="CQ58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS58" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ58" s="2"/>
+      <c r="CR58" s="2"/>
+      <c r="CS58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
@@ -17416,15 +17068,9 @@
       <c r="CP59" s="2" t="n">
         <v>0.85</v>
       </c>
-      <c r="CQ59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS59" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ59" s="2"/>
+      <c r="CR59" s="2"/>
+      <c r="CS59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
@@ -17709,15 +17355,9 @@
       <c r="CP60" s="2" t="n">
         <v>0.871</v>
       </c>
-      <c r="CQ60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS60" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ60" s="2"/>
+      <c r="CR60" s="2"/>
+      <c r="CS60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
@@ -18002,15 +17642,9 @@
       <c r="CP61" s="2" t="n">
         <v>0.891</v>
       </c>
-      <c r="CQ61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS61" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ61" s="2"/>
+      <c r="CR61" s="2"/>
+      <c r="CS61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
@@ -18295,15 +17929,9 @@
       <c r="CP62" s="2" t="n">
         <v>0.913</v>
       </c>
-      <c r="CQ62" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR62" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS62" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ62" s="2"/>
+      <c r="CR62" s="2"/>
+      <c r="CS62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
@@ -18588,15 +18216,9 @@
       <c r="CP63" s="2" t="n">
         <v>0.936</v>
       </c>
-      <c r="CQ63" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR63" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS63" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ63" s="2"/>
+      <c r="CR63" s="2"/>
+      <c r="CS63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
@@ -18881,15 +18503,9 @@
       <c r="CP64" s="2" t="n">
         <v>0.964</v>
       </c>
-      <c r="CQ64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS64" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ64" s="2"/>
+      <c r="CR64" s="2"/>
+      <c r="CS64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
@@ -19174,15 +18790,9 @@
       <c r="CP65" s="2" t="n">
         <v>0.976</v>
       </c>
-      <c r="CQ65" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR65" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS65" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ65" s="2"/>
+      <c r="CR65" s="2"/>
+      <c r="CS65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
@@ -19467,15 +19077,9 @@
       <c r="CP66" s="2" t="n">
         <v>0.999</v>
       </c>
-      <c r="CQ66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS66" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ66" s="2"/>
+      <c r="CR66" s="2"/>
+      <c r="CS66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
@@ -19760,15 +19364,9 @@
       <c r="CP67" s="2" t="n">
         <v>1.025</v>
       </c>
-      <c r="CQ67" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR67" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS67" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ67" s="2"/>
+      <c r="CR67" s="2"/>
+      <c r="CS67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
@@ -20053,15 +19651,9 @@
       <c r="CP68" s="2" t="n">
         <v>1.035</v>
       </c>
-      <c r="CQ68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS68" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ68" s="2"/>
+      <c r="CR68" s="2"/>
+      <c r="CS68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
@@ -20346,15 +19938,9 @@
       <c r="CP69" s="2" t="n">
         <v>1.057</v>
       </c>
-      <c r="CQ69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS69" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ69" s="2"/>
+      <c r="CR69" s="2"/>
+      <c r="CS69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
@@ -20639,15 +20225,9 @@
       <c r="CP70" s="2" t="n">
         <v>1.072</v>
       </c>
-      <c r="CQ70" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR70" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS70" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ70" s="2"/>
+      <c r="CR70" s="2"/>
+      <c r="CS70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
@@ -20932,15 +20512,9 @@
       <c r="CP71" s="2" t="n">
         <v>1.099</v>
       </c>
-      <c r="CQ71" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR71" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS71" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ71" s="2"/>
+      <c r="CR71" s="2"/>
+      <c r="CS71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
@@ -21225,15 +20799,9 @@
       <c r="CP72" s="2" t="n">
         <v>1.113</v>
       </c>
-      <c r="CQ72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS72" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ72" s="2"/>
+      <c r="CR72" s="2"/>
+      <c r="CS72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
@@ -21518,15 +21086,9 @@
       <c r="CP73" s="2" t="n">
         <v>1.133</v>
       </c>
-      <c r="CQ73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS73" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ73" s="2"/>
+      <c r="CR73" s="2"/>
+      <c r="CS73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
@@ -21811,15 +21373,9 @@
       <c r="CP74" s="2" t="n">
         <v>1.154</v>
       </c>
-      <c r="CQ74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS74" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ74" s="2"/>
+      <c r="CR74" s="2"/>
+      <c r="CS74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
@@ -22104,15 +21660,9 @@
       <c r="CP75" s="2" t="n">
         <v>1.173</v>
       </c>
-      <c r="CQ75" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR75" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS75" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ75" s="2"/>
+      <c r="CR75" s="2"/>
+      <c r="CS75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
@@ -22397,15 +21947,9 @@
       <c r="CP76" s="2" t="n">
         <v>1.19</v>
       </c>
-      <c r="CQ76" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR76" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS76" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ76" s="2"/>
+      <c r="CR76" s="2"/>
+      <c r="CS76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
@@ -22690,15 +22234,9 @@
       <c r="CP77" s="2" t="n">
         <v>1.217</v>
       </c>
-      <c r="CQ77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS77" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ77" s="2"/>
+      <c r="CR77" s="2"/>
+      <c r="CS77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
@@ -22983,15 +22521,9 @@
       <c r="CP78" s="2" t="n">
         <v>1.222</v>
       </c>
-      <c r="CQ78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS78" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ78" s="2"/>
+      <c r="CR78" s="2"/>
+      <c r="CS78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
@@ -23276,15 +22808,9 @@
       <c r="CP79" s="2" t="n">
         <v>1.248</v>
       </c>
-      <c r="CQ79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS79" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ79" s="2"/>
+      <c r="CR79" s="2"/>
+      <c r="CS79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -23569,15 +23095,9 @@
       <c r="CP80" s="2" t="n">
         <v>1.268</v>
       </c>
-      <c r="CQ80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS80" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ80" s="2"/>
+      <c r="CR80" s="2"/>
+      <c r="CS80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
@@ -23862,15 +23382,9 @@
       <c r="CP81" s="2" t="n">
         <v>1.294</v>
       </c>
-      <c r="CQ81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS81" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ81" s="2"/>
+      <c r="CR81" s="2"/>
+      <c r="CS81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
@@ -24155,15 +23669,9 @@
       <c r="CP82" s="2" t="n">
         <v>1.293</v>
       </c>
-      <c r="CQ82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS82" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ82" s="2"/>
+      <c r="CR82" s="2"/>
+      <c r="CS82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
@@ -24448,15 +23956,9 @@
       <c r="CP83" s="2" t="n">
         <v>1.32</v>
       </c>
-      <c r="CQ83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS83" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ83" s="2"/>
+      <c r="CR83" s="2"/>
+      <c r="CS83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
@@ -24741,15 +24243,9 @@
       <c r="CP84" s="2" t="n">
         <v>1.335</v>
       </c>
-      <c r="CQ84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS84" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ84" s="2"/>
+      <c r="CR84" s="2"/>
+      <c r="CS84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
@@ -25034,15 +24530,9 @@
       <c r="CP85" s="2" t="n">
         <v>1.352</v>
       </c>
-      <c r="CQ85" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR85" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS85" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ85" s="2"/>
+      <c r="CR85" s="2"/>
+      <c r="CS85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
@@ -25327,15 +24817,9 @@
       <c r="CP86" s="2" t="n">
         <v>1.357</v>
       </c>
-      <c r="CQ86" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR86" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS86" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ86" s="2"/>
+      <c r="CR86" s="2"/>
+      <c r="CS86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
@@ -25620,15 +25104,9 @@
       <c r="CP87" s="2" t="n">
         <v>1.375</v>
       </c>
-      <c r="CQ87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS87" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ87" s="2"/>
+      <c r="CR87" s="2"/>
+      <c r="CS87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
@@ -25913,15 +25391,9 @@
       <c r="CP88" s="2" t="n">
         <v>1.39</v>
       </c>
-      <c r="CQ88" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR88" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS88" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ88" s="2"/>
+      <c r="CR88" s="2"/>
+      <c r="CS88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
@@ -26206,15 +25678,9 @@
       <c r="CP89" s="2" t="n">
         <v>1.411</v>
       </c>
-      <c r="CQ89" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR89" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS89" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ89" s="2"/>
+      <c r="CR89" s="2"/>
+      <c r="CS89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
@@ -26499,15 +25965,9 @@
       <c r="CP90" s="2" t="n">
         <v>1.428</v>
       </c>
-      <c r="CQ90" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR90" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS90" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ90" s="2"/>
+      <c r="CR90" s="2"/>
+      <c r="CS90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -26792,15 +26252,9 @@
       <c r="CP91" s="2" t="n">
         <v>1.449</v>
       </c>
-      <c r="CQ91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS91" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ91" s="2"/>
+      <c r="CR91" s="2"/>
+      <c r="CS91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
@@ -27085,15 +26539,9 @@
       <c r="CP92" s="2" t="n">
         <v>1.469</v>
       </c>
-      <c r="CQ92" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR92" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS92" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ92" s="2"/>
+      <c r="CR92" s="2"/>
+      <c r="CS92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
@@ -27378,15 +26826,9 @@
       <c r="CP93" s="2" t="n">
         <v>1.479</v>
       </c>
-      <c r="CQ93" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR93" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS93" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ93" s="2"/>
+      <c r="CR93" s="2"/>
+      <c r="CS93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
@@ -27671,15 +27113,9 @@
       <c r="CP94" s="2" t="n">
         <v>1.498</v>
       </c>
-      <c r="CQ94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS94" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ94" s="2"/>
+      <c r="CR94" s="2"/>
+      <c r="CS94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
@@ -27964,15 +27400,9 @@
       <c r="CP95" s="2" t="n">
         <v>1.508</v>
       </c>
-      <c r="CQ95" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR95" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS95" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ95" s="2"/>
+      <c r="CR95" s="2"/>
+      <c r="CS95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
@@ -28257,15 +27687,9 @@
       <c r="CP96" s="2" t="n">
         <v>1.536</v>
       </c>
-      <c r="CQ96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS96" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ96" s="2"/>
+      <c r="CR96" s="2"/>
+      <c r="CS96" s="2"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
@@ -28550,15 +27974,9 @@
       <c r="CP97" s="2" t="n">
         <v>1.547</v>
       </c>
-      <c r="CQ97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS97" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ97" s="2"/>
+      <c r="CR97" s="2"/>
+      <c r="CS97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
@@ -28843,15 +28261,9 @@
       <c r="CP98" s="2" t="n">
         <v>1.573</v>
       </c>
-      <c r="CQ98" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR98" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS98" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ98" s="2"/>
+      <c r="CR98" s="2"/>
+      <c r="CS98" s="2"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
@@ -29136,15 +28548,9 @@
       <c r="CP99" s="2" t="n">
         <v>1.585</v>
       </c>
-      <c r="CQ99" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR99" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS99" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ99" s="2"/>
+      <c r="CR99" s="2"/>
+      <c r="CS99" s="2"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
@@ -29429,15 +28835,9 @@
       <c r="CP100" s="2" t="n">
         <v>1.598</v>
       </c>
-      <c r="CQ100" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR100" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS100" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ100" s="2"/>
+      <c r="CR100" s="2"/>
+      <c r="CS100" s="2"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
@@ -29722,15 +29122,9 @@
       <c r="CP101" s="2" t="n">
         <v>1.613</v>
       </c>
-      <c r="CQ101" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR101" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS101" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ101" s="2"/>
+      <c r="CR101" s="2"/>
+      <c r="CS101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
@@ -30015,15 +29409,9 @@
       <c r="CP102" s="2" t="n">
         <v>1.643</v>
       </c>
-      <c r="CQ102" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR102" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS102" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ102" s="2"/>
+      <c r="CR102" s="2"/>
+      <c r="CS102" s="2"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="n">
@@ -30308,15 +29696,9 @@
       <c r="CP103" s="2" t="n">
         <v>1.658</v>
       </c>
-      <c r="CQ103" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR103" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS103" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ103" s="2"/>
+      <c r="CR103" s="2"/>
+      <c r="CS103" s="2"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="n">
@@ -30601,15 +29983,9 @@
       <c r="CP104" s="2" t="n">
         <v>1.663</v>
       </c>
-      <c r="CQ104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS104" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ104" s="2"/>
+      <c r="CR104" s="2"/>
+      <c r="CS104" s="2"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="n">
@@ -30894,15 +30270,9 @@
       <c r="CP105" s="2" t="n">
         <v>1.7</v>
       </c>
-      <c r="CQ105" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR105" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS105" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ105" s="2"/>
+      <c r="CR105" s="2"/>
+      <c r="CS105" s="2"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="n">
@@ -31187,15 +30557,9 @@
       <c r="CP106" s="2" t="n">
         <v>1.705</v>
       </c>
-      <c r="CQ106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS106" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ106" s="2"/>
+      <c r="CR106" s="2"/>
+      <c r="CS106" s="2"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="n">
@@ -31480,15 +30844,9 @@
       <c r="CP107" s="2" t="n">
         <v>1.716</v>
       </c>
-      <c r="CQ107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS107" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ107" s="2"/>
+      <c r="CR107" s="2"/>
+      <c r="CS107" s="2"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="n">
@@ -31773,15 +31131,9 @@
       <c r="CP108" s="2" t="n">
         <v>1.74</v>
       </c>
-      <c r="CQ108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS108" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ108" s="2"/>
+      <c r="CR108" s="2"/>
+      <c r="CS108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="n">
@@ -32066,15 +31418,9 @@
       <c r="CP109" s="2" t="n">
         <v>1.742</v>
       </c>
-      <c r="CQ109" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR109" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS109" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ109" s="2"/>
+      <c r="CR109" s="2"/>
+      <c r="CS109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="n">
@@ -32359,15 +31705,9 @@
       <c r="CP110" s="2" t="n">
         <v>1.762</v>
       </c>
-      <c r="CQ110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS110" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ110" s="2"/>
+      <c r="CR110" s="2"/>
+      <c r="CS110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="n">
@@ -32652,15 +31992,9 @@
       <c r="CP111" s="2" t="n">
         <v>1.781</v>
       </c>
-      <c r="CQ111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS111" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ111" s="2"/>
+      <c r="CR111" s="2"/>
+      <c r="CS111" s="2"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="n">
@@ -32945,15 +32279,9 @@
       <c r="CP112" s="2" t="n">
         <v>1.783</v>
       </c>
-      <c r="CQ112" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR112" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS112" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ112" s="2"/>
+      <c r="CR112" s="2"/>
+      <c r="CS112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="n">
@@ -33238,15 +32566,9 @@
       <c r="CP113" s="2" t="n">
         <v>1.806</v>
       </c>
-      <c r="CQ113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS113" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ113" s="2"/>
+      <c r="CR113" s="2"/>
+      <c r="CS113" s="2"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="n">
@@ -33531,15 +32853,9 @@
       <c r="CP114" s="2" t="n">
         <v>1.817</v>
       </c>
-      <c r="CQ114" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR114" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS114" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ114" s="2"/>
+      <c r="CR114" s="2"/>
+      <c r="CS114" s="2"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="n">
@@ -33824,15 +33140,9 @@
       <c r="CP115" s="2" t="n">
         <v>1.842</v>
       </c>
-      <c r="CQ115" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR115" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS115" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ115" s="2"/>
+      <c r="CR115" s="2"/>
+      <c r="CS115" s="2"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="n">
@@ -34117,15 +33427,9 @@
       <c r="CP116" s="2" t="n">
         <v>1.851</v>
       </c>
-      <c r="CQ116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS116" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ116" s="2"/>
+      <c r="CR116" s="2"/>
+      <c r="CS116" s="2"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="n">
@@ -34410,15 +33714,9 @@
       <c r="CP117" s="2" t="n">
         <v>1.87</v>
       </c>
-      <c r="CQ117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS117" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ117" s="2"/>
+      <c r="CR117" s="2"/>
+      <c r="CS117" s="2"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="n">
@@ -34703,15 +34001,9 @@
       <c r="CP118" s="2" t="n">
         <v>1.881</v>
       </c>
-      <c r="CQ118" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR118" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS118" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ118" s="2"/>
+      <c r="CR118" s="2"/>
+      <c r="CS118" s="2"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="n">
@@ -34996,15 +34288,9 @@
       <c r="CP119" s="2" t="n">
         <v>1.913</v>
       </c>
-      <c r="CQ119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS119" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ119" s="2"/>
+      <c r="CR119" s="2"/>
+      <c r="CS119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="n">
@@ -35289,15 +34575,9 @@
       <c r="CP120" s="2" t="n">
         <v>1.905</v>
       </c>
-      <c r="CQ120" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR120" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS120" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ120" s="2"/>
+      <c r="CR120" s="2"/>
+      <c r="CS120" s="2"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="n">
@@ -35582,15 +34862,9 @@
       <c r="CP121" s="2" t="n">
         <v>1.921</v>
       </c>
-      <c r="CQ121" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR121" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS121" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ121" s="2"/>
+      <c r="CR121" s="2"/>
+      <c r="CS121" s="2"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="n">
@@ -35875,15 +35149,9 @@
       <c r="CP122" s="2" t="n">
         <v>1.936</v>
       </c>
-      <c r="CQ122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS122" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ122" s="2"/>
+      <c r="CR122" s="2"/>
+      <c r="CS122" s="2"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="n">
@@ -36168,15 +35436,9 @@
       <c r="CP123" s="2" t="n">
         <v>1.948</v>
       </c>
-      <c r="CQ123" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR123" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS123" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ123" s="2"/>
+      <c r="CR123" s="2"/>
+      <c r="CS123" s="2"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="n">
@@ -36461,15 +35723,9 @@
       <c r="CP124" s="2" t="n">
         <v>1.967</v>
       </c>
-      <c r="CQ124" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR124" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS124" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ124" s="2"/>
+      <c r="CR124" s="2"/>
+      <c r="CS124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="n">
@@ -36754,15 +36010,9 @@
       <c r="CP125" s="2" t="n">
         <v>1.973</v>
       </c>
-      <c r="CQ125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS125" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ125" s="2"/>
+      <c r="CR125" s="2"/>
+      <c r="CS125" s="2"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="n">
@@ -37047,15 +36297,9 @@
       <c r="CP126" s="2" t="n">
         <v>1.981</v>
       </c>
-      <c r="CQ126" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR126" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS126" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ126" s="2"/>
+      <c r="CR126" s="2"/>
+      <c r="CS126" s="2"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="n">
@@ -37340,15 +36584,9 @@
       <c r="CP127" s="2" t="n">
         <v>2.015</v>
       </c>
-      <c r="CQ127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS127" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ127" s="2"/>
+      <c r="CR127" s="2"/>
+      <c r="CS127" s="2"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="n">
@@ -37633,15 +36871,9 @@
       <c r="CP128" s="2" t="n">
         <v>2.029</v>
       </c>
-      <c r="CQ128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS128" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ128" s="2"/>
+      <c r="CR128" s="2"/>
+      <c r="CS128" s="2"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="n">
@@ -37926,15 +37158,9 @@
       <c r="CP129" s="2" t="n">
         <v>2.062</v>
       </c>
-      <c r="CQ129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS129" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ129" s="2"/>
+      <c r="CR129" s="2"/>
+      <c r="CS129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="n">
@@ -38219,15 +37445,9 @@
       <c r="CP130" s="2" t="n">
         <v>2.076</v>
       </c>
-      <c r="CQ130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS130" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ130" s="2"/>
+      <c r="CR130" s="2"/>
+      <c r="CS130" s="2"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="n">
@@ -38512,15 +37732,9 @@
       <c r="CP131" s="2" t="n">
         <v>2.103</v>
       </c>
-      <c r="CQ131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS131" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ131" s="2"/>
+      <c r="CR131" s="2"/>
+      <c r="CS131" s="2"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="n">
@@ -38805,15 +38019,9 @@
       <c r="CP132" s="2" t="n">
         <v>2.106</v>
       </c>
-      <c r="CQ132" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR132" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS132" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ132" s="2"/>
+      <c r="CR132" s="2"/>
+      <c r="CS132" s="2"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="n">
@@ -39098,15 +38306,9 @@
       <c r="CP133" s="2" t="n">
         <v>2.122</v>
       </c>
-      <c r="CQ133" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR133" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS133" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ133" s="2"/>
+      <c r="CR133" s="2"/>
+      <c r="CS133" s="2"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="n">
@@ -39391,15 +38593,9 @@
       <c r="CP134" s="2" t="n">
         <v>2.138</v>
       </c>
-      <c r="CQ134" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR134" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS134" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ134" s="2"/>
+      <c r="CR134" s="2"/>
+      <c r="CS134" s="2"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="n">
@@ -39684,15 +38880,9 @@
       <c r="CP135" s="2" t="n">
         <v>2.16</v>
       </c>
-      <c r="CQ135" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR135" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS135" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ135" s="2"/>
+      <c r="CR135" s="2"/>
+      <c r="CS135" s="2"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="n">
@@ -39977,15 +39167,9 @@
       <c r="CP136" s="2" t="n">
         <v>2.161</v>
       </c>
-      <c r="CQ136" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR136" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS136" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ136" s="2"/>
+      <c r="CR136" s="2"/>
+      <c r="CS136" s="2"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="n">
@@ -40270,15 +39454,9 @@
       <c r="CP137" s="2" t="n">
         <v>2.171</v>
       </c>
-      <c r="CQ137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS137" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ137" s="2"/>
+      <c r="CR137" s="2"/>
+      <c r="CS137" s="2"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="n">
@@ -40563,15 +39741,9 @@
       <c r="CP138" s="2" t="n">
         <v>2.198</v>
       </c>
-      <c r="CQ138" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR138" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS138" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ138" s="2"/>
+      <c r="CR138" s="2"/>
+      <c r="CS138" s="2"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="n">
@@ -40856,15 +40028,9 @@
       <c r="CP139" s="2" t="n">
         <v>2.211</v>
       </c>
-      <c r="CQ139" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR139" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS139" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ139" s="2"/>
+      <c r="CR139" s="2"/>
+      <c r="CS139" s="2"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="n">
@@ -41149,15 +40315,9 @@
       <c r="CP140" s="2" t="n">
         <v>2.222</v>
       </c>
-      <c r="CQ140" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR140" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS140" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ140" s="2"/>
+      <c r="CR140" s="2"/>
+      <c r="CS140" s="2"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="n">
@@ -41442,15 +40602,9 @@
       <c r="CP141" s="2" t="n">
         <v>2.229</v>
       </c>
-      <c r="CQ141" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR141" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS141" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ141" s="2"/>
+      <c r="CR141" s="2"/>
+      <c r="CS141" s="2"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="n">
@@ -41735,15 +40889,9 @@
       <c r="CP142" s="2" t="n">
         <v>2.248</v>
       </c>
-      <c r="CQ142" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR142" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS142" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ142" s="2"/>
+      <c r="CR142" s="2"/>
+      <c r="CS142" s="2"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="n">
@@ -42028,15 +41176,9 @@
       <c r="CP143" s="2" t="n">
         <v>2.25</v>
       </c>
-      <c r="CQ143" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR143" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS143" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ143" s="2"/>
+      <c r="CR143" s="2"/>
+      <c r="CS143" s="2"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="n">
@@ -42321,15 +41463,9 @@
       <c r="CP144" s="2" t="n">
         <v>2.266</v>
       </c>
-      <c r="CQ144" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR144" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS144" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ144" s="2"/>
+      <c r="CR144" s="2"/>
+      <c r="CS144" s="2"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="n">
@@ -42614,15 +41750,9 @@
       <c r="CP145" s="2" t="n">
         <v>2.286</v>
       </c>
-      <c r="CQ145" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR145" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS145" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ145" s="2"/>
+      <c r="CR145" s="2"/>
+      <c r="CS145" s="2"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="n">
@@ -42907,15 +42037,9 @@
       <c r="CP146" s="2" t="n">
         <v>2.284</v>
       </c>
-      <c r="CQ146" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR146" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS146" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ146" s="2"/>
+      <c r="CR146" s="2"/>
+      <c r="CS146" s="2"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="n">
@@ -43200,15 +42324,9 @@
       <c r="CP147" s="2" t="n">
         <v>2.298</v>
       </c>
-      <c r="CQ147" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR147" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS147" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ147" s="2"/>
+      <c r="CR147" s="2"/>
+      <c r="CS147" s="2"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="n">
@@ -43493,15 +42611,9 @@
       <c r="CP148" s="2" t="n">
         <v>2.316</v>
       </c>
-      <c r="CQ148" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR148" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS148" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ148" s="2"/>
+      <c r="CR148" s="2"/>
+      <c r="CS148" s="2"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="n">
@@ -43786,15 +42898,9 @@
       <c r="CP149" s="2" t="n">
         <v>2.332</v>
       </c>
-      <c r="CQ149" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR149" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS149" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ149" s="2"/>
+      <c r="CR149" s="2"/>
+      <c r="CS149" s="2"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="n">
@@ -44079,15 +43185,9 @@
       <c r="CP150" s="2" t="n">
         <v>2.343</v>
       </c>
-      <c r="CQ150" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR150" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS150" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ150" s="2"/>
+      <c r="CR150" s="2"/>
+      <c r="CS150" s="2"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="n">
@@ -44372,15 +43472,9 @@
       <c r="CP151" s="2" t="n">
         <v>2.36</v>
       </c>
-      <c r="CQ151" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR151" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS151" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ151" s="2"/>
+      <c r="CR151" s="2"/>
+      <c r="CS151" s="2"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="n">
@@ -44665,15 +43759,9 @@
       <c r="CP152" s="2" t="n">
         <v>2.362</v>
       </c>
-      <c r="CQ152" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR152" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS152" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ152" s="2"/>
+      <c r="CR152" s="2"/>
+      <c r="CS152" s="2"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="n">
@@ -44958,15 +44046,9 @@
       <c r="CP153" s="2" t="n">
         <v>2.39</v>
       </c>
-      <c r="CQ153" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR153" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS153" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ153" s="2"/>
+      <c r="CR153" s="2"/>
+      <c r="CS153" s="2"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="n">
@@ -45251,15 +44333,9 @@
       <c r="CP154" s="2" t="n">
         <v>2.403</v>
       </c>
-      <c r="CQ154" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR154" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS154" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ154" s="2"/>
+      <c r="CR154" s="2"/>
+      <c r="CS154" s="2"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="n">
@@ -45544,15 +44620,9 @@
       <c r="CP155" s="2" t="n">
         <v>2.413</v>
       </c>
-      <c r="CQ155" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR155" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS155" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ155" s="2"/>
+      <c r="CR155" s="2"/>
+      <c r="CS155" s="2"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="n">
@@ -45837,15 +44907,9 @@
       <c r="CP156" s="2" t="n">
         <v>2.435</v>
       </c>
-      <c r="CQ156" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR156" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS156" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ156" s="2"/>
+      <c r="CR156" s="2"/>
+      <c r="CS156" s="2"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="n">
@@ -46130,15 +45194,9 @@
       <c r="CP157" s="2" t="n">
         <v>2.447</v>
       </c>
-      <c r="CQ157" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR157" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS157" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ157" s="2"/>
+      <c r="CR157" s="2"/>
+      <c r="CS157" s="2"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="n">
@@ -46423,15 +45481,9 @@
       <c r="CP158" s="2" t="n">
         <v>2.459</v>
       </c>
-      <c r="CQ158" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR158" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS158" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ158" s="2"/>
+      <c r="CR158" s="2"/>
+      <c r="CS158" s="2"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="n">
@@ -46716,15 +45768,9 @@
       <c r="CP159" s="2" t="n">
         <v>2.471</v>
       </c>
-      <c r="CQ159" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR159" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS159" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ159" s="2"/>
+      <c r="CR159" s="2"/>
+      <c r="CS159" s="2"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="n">
@@ -47009,15 +46055,9 @@
       <c r="CP160" s="2" t="n">
         <v>2.502</v>
       </c>
-      <c r="CQ160" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR160" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS160" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ160" s="2"/>
+      <c r="CR160" s="2"/>
+      <c r="CS160" s="2"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="n">
@@ -47302,15 +46342,9 @@
       <c r="CP161" s="2" t="n">
         <v>2.505</v>
       </c>
-      <c r="CQ161" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR161" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS161" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ161" s="2"/>
+      <c r="CR161" s="2"/>
+      <c r="CS161" s="2"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="n">
@@ -47595,15 +46629,9 @@
       <c r="CP162" s="2" t="n">
         <v>2.512</v>
       </c>
-      <c r="CQ162" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR162" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS162" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ162" s="2"/>
+      <c r="CR162" s="2"/>
+      <c r="CS162" s="2"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="n">
@@ -47888,15 +46916,9 @@
       <c r="CP163" s="2" t="n">
         <v>2.532</v>
       </c>
-      <c r="CQ163" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR163" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS163" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ163" s="2"/>
+      <c r="CR163" s="2"/>
+      <c r="CS163" s="2"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="n">
@@ -48181,15 +47203,9 @@
       <c r="CP164" s="2" t="n">
         <v>2.546</v>
       </c>
-      <c r="CQ164" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR164" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS164" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ164" s="2"/>
+      <c r="CR164" s="2"/>
+      <c r="CS164" s="2"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="n">
@@ -48474,15 +47490,9 @@
       <c r="CP165" s="2" t="n">
         <v>2.553</v>
       </c>
-      <c r="CQ165" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR165" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS165" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ165" s="2"/>
+      <c r="CR165" s="2"/>
+      <c r="CS165" s="2"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="n">
@@ -48767,15 +47777,9 @@
       <c r="CP166" s="2" t="n">
         <v>2.57</v>
       </c>
-      <c r="CQ166" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR166" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS166" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ166" s="2"/>
+      <c r="CR166" s="2"/>
+      <c r="CS166" s="2"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="n">
@@ -49060,15 +48064,9 @@
       <c r="CP167" s="2" t="n">
         <v>2.571</v>
       </c>
-      <c r="CQ167" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR167" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS167" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ167" s="2"/>
+      <c r="CR167" s="2"/>
+      <c r="CS167" s="2"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="n">
@@ -49353,15 +48351,9 @@
       <c r="CP168" s="2" t="n">
         <v>2.585</v>
       </c>
-      <c r="CQ168" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR168" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS168" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ168" s="2"/>
+      <c r="CR168" s="2"/>
+      <c r="CS168" s="2"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="n">
@@ -49646,15 +48638,9 @@
       <c r="CP169" s="2" t="n">
         <v>2.605</v>
       </c>
-      <c r="CQ169" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR169" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS169" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ169" s="2"/>
+      <c r="CR169" s="2"/>
+      <c r="CS169" s="2"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="n">
@@ -49939,15 +48925,9 @@
       <c r="CP170" s="2" t="n">
         <v>2.593</v>
       </c>
-      <c r="CQ170" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR170" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS170" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ170" s="2"/>
+      <c r="CR170" s="2"/>
+      <c r="CS170" s="2"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="n">
@@ -50232,15 +49212,9 @@
       <c r="CP171" s="2" t="n">
         <v>2.63</v>
       </c>
-      <c r="CQ171" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR171" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS171" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ171" s="2"/>
+      <c r="CR171" s="2"/>
+      <c r="CS171" s="2"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="n">
@@ -50525,15 +49499,9 @@
       <c r="CP172" s="2" t="n">
         <v>2.639</v>
       </c>
-      <c r="CQ172" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR172" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS172" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ172" s="2"/>
+      <c r="CR172" s="2"/>
+      <c r="CS172" s="2"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="n">
@@ -50818,15 +49786,9 @@
       <c r="CP173" s="2" t="n">
         <v>2.65</v>
       </c>
-      <c r="CQ173" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR173" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS173" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ173" s="2"/>
+      <c r="CR173" s="2"/>
+      <c r="CS173" s="2"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="n">
@@ -51111,15 +50073,9 @@
       <c r="CP174" s="2" t="n">
         <v>2.666</v>
       </c>
-      <c r="CQ174" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR174" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS174" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ174" s="2"/>
+      <c r="CR174" s="2"/>
+      <c r="CS174" s="2"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="n">
@@ -51404,15 +50360,9 @@
       <c r="CP175" s="2" t="n">
         <v>2.694</v>
       </c>
-      <c r="CQ175" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR175" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS175" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ175" s="2"/>
+      <c r="CR175" s="2"/>
+      <c r="CS175" s="2"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="n">
@@ -51697,15 +50647,9 @@
       <c r="CP176" s="2" t="n">
         <v>2.694</v>
       </c>
-      <c r="CQ176" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR176" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS176" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ176" s="2"/>
+      <c r="CR176" s="2"/>
+      <c r="CS176" s="2"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="n">
@@ -51990,15 +50934,9 @@
       <c r="CP177" s="2" t="n">
         <v>2.711</v>
       </c>
-      <c r="CQ177" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR177" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS177" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ177" s="2"/>
+      <c r="CR177" s="2"/>
+      <c r="CS177" s="2"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="n">
@@ -52283,15 +51221,9 @@
       <c r="CP178" s="2" t="n">
         <v>2.728</v>
       </c>
-      <c r="CQ178" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR178" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS178" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ178" s="2"/>
+      <c r="CR178" s="2"/>
+      <c r="CS178" s="2"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="n">
@@ -52576,15 +51508,9 @@
       <c r="CP179" s="2" t="n">
         <v>2.755</v>
       </c>
-      <c r="CQ179" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR179" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS179" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ179" s="2"/>
+      <c r="CR179" s="2"/>
+      <c r="CS179" s="2"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="n">
@@ -52869,15 +51795,9 @@
       <c r="CP180" s="2" t="n">
         <v>2.76</v>
       </c>
-      <c r="CQ180" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR180" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS180" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ180" s="2"/>
+      <c r="CR180" s="2"/>
+      <c r="CS180" s="2"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="n">
@@ -53162,15 +52082,9 @@
       <c r="CP181" s="2" t="n">
         <v>2.771</v>
       </c>
-      <c r="CQ181" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR181" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS181" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ181" s="2"/>
+      <c r="CR181" s="2"/>
+      <c r="CS181" s="2"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="n">
@@ -53455,15 +52369,9 @@
       <c r="CP182" s="2" t="n">
         <v>2.793</v>
       </c>
-      <c r="CQ182" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR182" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS182" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ182" s="2"/>
+      <c r="CR182" s="2"/>
+      <c r="CS182" s="2"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="n">
@@ -53748,15 +52656,9 @@
       <c r="CP183" s="2" t="n">
         <v>2.799</v>
       </c>
-      <c r="CQ183" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR183" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS183" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ183" s="2"/>
+      <c r="CR183" s="2"/>
+      <c r="CS183" s="2"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="n">
@@ -54041,15 +52943,9 @@
       <c r="CP184" s="2" t="n">
         <v>2.821</v>
       </c>
-      <c r="CQ184" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR184" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS184" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ184" s="2"/>
+      <c r="CR184" s="2"/>
+      <c r="CS184" s="2"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="n">
@@ -54334,15 +53230,9 @@
       <c r="CP185" s="2" t="n">
         <v>2.88</v>
       </c>
-      <c r="CQ185" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR185" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS185" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ185" s="2"/>
+      <c r="CR185" s="2"/>
+      <c r="CS185" s="2"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="n">
@@ -54627,15 +53517,9 @@
       <c r="CP186" s="2" t="n">
         <v>2.858</v>
       </c>
-      <c r="CQ186" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR186" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS186" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ186" s="2"/>
+      <c r="CR186" s="2"/>
+      <c r="CS186" s="2"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="n">
@@ -54920,15 +53804,9 @@
       <c r="CP187" s="2" t="n">
         <v>2.885</v>
       </c>
-      <c r="CQ187" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR187" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS187" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ187" s="2"/>
+      <c r="CR187" s="2"/>
+      <c r="CS187" s="2"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="n">
@@ -55213,15 +54091,9 @@
       <c r="CP188" s="2" t="n">
         <v>2.89</v>
       </c>
-      <c r="CQ188" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR188" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS188" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ188" s="2"/>
+      <c r="CR188" s="2"/>
+      <c r="CS188" s="2"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="n">
@@ -55506,15 +54378,9 @@
       <c r="CP189" s="2" t="n">
         <v>2.958</v>
       </c>
-      <c r="CQ189" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR189" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS189" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ189" s="2"/>
+      <c r="CR189" s="2"/>
+      <c r="CS189" s="2"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="n">
@@ -55799,15 +54665,9 @@
       <c r="CP190" s="2" t="n">
         <v>2.908</v>
       </c>
-      <c r="CQ190" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR190" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS190" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ190" s="2"/>
+      <c r="CR190" s="2"/>
+      <c r="CS190" s="2"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="n">
@@ -56092,15 +54952,9 @@
       <c r="CP191" s="2" t="n">
         <v>2.93</v>
       </c>
-      <c r="CQ191" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR191" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS191" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ191" s="2"/>
+      <c r="CR191" s="2"/>
+      <c r="CS191" s="2"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="n">
@@ -56385,15 +55239,9 @@
       <c r="CP192" s="2" t="n">
         <v>2.968</v>
       </c>
-      <c r="CQ192" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR192" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS192" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ192" s="2"/>
+      <c r="CR192" s="2"/>
+      <c r="CS192" s="2"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="n">
@@ -56678,15 +55526,9 @@
       <c r="CP193" s="2" t="n">
         <v>2.968</v>
       </c>
-      <c r="CQ193" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR193" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS193" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ193" s="2"/>
+      <c r="CR193" s="2"/>
+      <c r="CS193" s="2"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="n">
@@ -56971,15 +55813,9 @@
       <c r="CP194" s="2" t="n">
         <v>2.993</v>
       </c>
-      <c r="CQ194" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR194" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS194" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ194" s="2"/>
+      <c r="CR194" s="2"/>
+      <c r="CS194" s="2"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="n">
@@ -57264,15 +56100,9 @@
       <c r="CP195" s="2" t="n">
         <v>3.009</v>
       </c>
-      <c r="CQ195" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR195" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS195" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ195" s="2"/>
+      <c r="CR195" s="2"/>
+      <c r="CS195" s="2"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="n">
@@ -57557,15 +56387,9 @@
       <c r="CP196" s="2" t="n">
         <v>3.038</v>
       </c>
-      <c r="CQ196" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR196" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS196" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ196" s="2"/>
+      <c r="CR196" s="2"/>
+      <c r="CS196" s="2"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="n">
@@ -57850,15 +56674,9 @@
       <c r="CP197" s="2" t="n">
         <v>3.067</v>
       </c>
-      <c r="CQ197" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR197" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS197" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ197" s="2"/>
+      <c r="CR197" s="2"/>
+      <c r="CS197" s="2"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="n">
@@ -58143,15 +56961,9 @@
       <c r="CP198" s="2" t="n">
         <v>3.063</v>
       </c>
-      <c r="CQ198" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR198" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS198" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ198" s="2"/>
+      <c r="CR198" s="2"/>
+      <c r="CS198" s="2"/>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="n">
@@ -58436,15 +57248,9 @@
       <c r="CP199" s="2" t="n">
         <v>3.095</v>
       </c>
-      <c r="CQ199" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR199" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS199" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ199" s="2"/>
+      <c r="CR199" s="2"/>
+      <c r="CS199" s="2"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="n">
@@ -58729,15 +57535,9 @@
       <c r="CP200" s="2" t="n">
         <v>3.11</v>
       </c>
-      <c r="CQ200" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR200" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS200" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ200" s="2"/>
+      <c r="CR200" s="2"/>
+      <c r="CS200" s="2"/>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="n">
@@ -59022,15 +57822,9 @@
       <c r="CP201" s="2" t="n">
         <v>3.128</v>
       </c>
-      <c r="CQ201" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR201" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS201" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ201" s="2"/>
+      <c r="CR201" s="2"/>
+      <c r="CS201" s="2"/>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="n">
@@ -59315,15 +58109,9 @@
       <c r="CP202" s="2" t="n">
         <v>3.141</v>
       </c>
-      <c r="CQ202" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR202" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS202" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ202" s="2"/>
+      <c r="CR202" s="2"/>
+      <c r="CS202" s="2"/>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="n">
@@ -59608,15 +58396,9 @@
       <c r="CP203" s="2" t="n">
         <v>3.179</v>
       </c>
-      <c r="CQ203" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR203" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS203" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ203" s="2"/>
+      <c r="CR203" s="2"/>
+      <c r="CS203" s="2"/>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="n">
@@ -59901,15 +58683,9 @@
       <c r="CP204" s="2" t="n">
         <v>3.203</v>
       </c>
-      <c r="CQ204" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR204" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS204" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ204" s="2"/>
+      <c r="CR204" s="2"/>
+      <c r="CS204" s="2"/>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="n">
@@ -60194,15 +58970,9 @@
       <c r="CP205" s="2" t="n">
         <v>3.217</v>
       </c>
-      <c r="CQ205" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR205" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS205" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ205" s="2"/>
+      <c r="CR205" s="2"/>
+      <c r="CS205" s="2"/>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="n">
@@ -60487,15 +59257,9 @@
       <c r="CP206" s="2" t="n">
         <v>3.239</v>
       </c>
-      <c r="CQ206" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR206" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS206" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ206" s="2"/>
+      <c r="CR206" s="2"/>
+      <c r="CS206" s="2"/>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="n">
@@ -60780,15 +59544,9 @@
       <c r="CP207" s="2" t="n">
         <v>3.263</v>
       </c>
-      <c r="CQ207" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR207" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS207" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ207" s="2"/>
+      <c r="CR207" s="2"/>
+      <c r="CS207" s="2"/>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="n">
@@ -61073,15 +59831,9 @@
       <c r="CP208" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="CQ208" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR208" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS208" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ208" s="2"/>
+      <c r="CR208" s="2"/>
+      <c r="CS208" s="2"/>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="n">
@@ -61366,15 +60118,9 @@
       <c r="CP209" s="2" t="n">
         <v>3.318</v>
       </c>
-      <c r="CQ209" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR209" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS209" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ209" s="2"/>
+      <c r="CR209" s="2"/>
+      <c r="CS209" s="2"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="n">
@@ -61659,15 +60405,9 @@
       <c r="CP210" s="2" t="n">
         <v>3.326</v>
       </c>
-      <c r="CQ210" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR210" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS210" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ210" s="2"/>
+      <c r="CR210" s="2"/>
+      <c r="CS210" s="2"/>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="n">
@@ -61952,15 +60692,9 @@
       <c r="CP211" s="2" t="n">
         <v>3.364</v>
       </c>
-      <c r="CQ211" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR211" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS211" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ211" s="2"/>
+      <c r="CR211" s="2"/>
+      <c r="CS211" s="2"/>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="n">
@@ -62245,15 +60979,9 @@
       <c r="CP212" s="2" t="n">
         <v>3.37</v>
       </c>
-      <c r="CQ212" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR212" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS212" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ212" s="2"/>
+      <c r="CR212" s="2"/>
+      <c r="CS212" s="2"/>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="n">
@@ -62538,15 +61266,9 @@
       <c r="CP213" s="2" t="n">
         <v>3.399</v>
       </c>
-      <c r="CQ213" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR213" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS213" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ213" s="2"/>
+      <c r="CR213" s="2"/>
+      <c r="CS213" s="2"/>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="n">
@@ -62831,15 +61553,9 @@
       <c r="CP214" s="2" t="n">
         <v>3.414</v>
       </c>
-      <c r="CQ214" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR214" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS214" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ214" s="2"/>
+      <c r="CR214" s="2"/>
+      <c r="CS214" s="2"/>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="n">
@@ -63124,15 +61840,9 @@
       <c r="CP215" s="2" t="n">
         <v>3.435</v>
       </c>
-      <c r="CQ215" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR215" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS215" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ215" s="2"/>
+      <c r="CR215" s="2"/>
+      <c r="CS215" s="2"/>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="n">
@@ -63417,15 +62127,9 @@
       <c r="CP216" s="2" t="n">
         <v>3.451</v>
       </c>
-      <c r="CQ216" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR216" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS216" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ216" s="2"/>
+      <c r="CR216" s="2"/>
+      <c r="CS216" s="2"/>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="n">
@@ -63710,15 +62414,9 @@
       <c r="CP217" s="2" t="n">
         <v>3.476</v>
       </c>
-      <c r="CQ217" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR217" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS217" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ217" s="2"/>
+      <c r="CR217" s="2"/>
+      <c r="CS217" s="2"/>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="n">
@@ -64003,15 +62701,9 @@
       <c r="CP218" s="2" t="n">
         <v>3.488</v>
       </c>
-      <c r="CQ218" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR218" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS218" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ218" s="2"/>
+      <c r="CR218" s="2"/>
+      <c r="CS218" s="2"/>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="n">
@@ -64296,15 +62988,9 @@
       <c r="CP219" s="2" t="n">
         <v>3.508</v>
       </c>
-      <c r="CQ219" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR219" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS219" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ219" s="2"/>
+      <c r="CR219" s="2"/>
+      <c r="CS219" s="2"/>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="n">
@@ -64589,15 +63275,9 @@
       <c r="CP220" s="2" t="n">
         <v>3.585</v>
       </c>
-      <c r="CQ220" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR220" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS220" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ220" s="2"/>
+      <c r="CR220" s="2"/>
+      <c r="CS220" s="2"/>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="n">
@@ -64882,15 +63562,9 @@
       <c r="CP221" s="2" t="n">
         <v>3.552</v>
       </c>
-      <c r="CQ221" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR221" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS221" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ221" s="2"/>
+      <c r="CR221" s="2"/>
+      <c r="CS221" s="2"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="n">
@@ -65175,15 +63849,9 @@
       <c r="CP222" s="2" t="n">
         <v>3.594</v>
       </c>
-      <c r="CQ222" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR222" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS222" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ222" s="2"/>
+      <c r="CR222" s="2"/>
+      <c r="CS222" s="2"/>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="n">
@@ -65468,15 +64136,9 @@
       <c r="CP223" s="2" t="n">
         <v>3.66</v>
       </c>
-      <c r="CQ223" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR223" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS223" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ223" s="2"/>
+      <c r="CR223" s="2"/>
+      <c r="CS223" s="2"/>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="n">
@@ -65761,15 +64423,9 @@
       <c r="CP224" s="2" t="n">
         <v>3.676</v>
       </c>
-      <c r="CQ224" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR224" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS224" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ224" s="2"/>
+      <c r="CR224" s="2"/>
+      <c r="CS224" s="2"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="n">
@@ -66054,15 +64710,9 @@
       <c r="CP225" s="2" t="n">
         <v>3.629</v>
       </c>
-      <c r="CQ225" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR225" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS225" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ225" s="2"/>
+      <c r="CR225" s="2"/>
+      <c r="CS225" s="2"/>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="n">
@@ -66347,15 +64997,9 @@
       <c r="CP226" s="2" t="n">
         <v>3.648</v>
       </c>
-      <c r="CQ226" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR226" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS226" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ226" s="2"/>
+      <c r="CR226" s="2"/>
+      <c r="CS226" s="2"/>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="n">
@@ -66640,15 +65284,9 @@
       <c r="CP227" s="2" t="n">
         <v>3.672</v>
       </c>
-      <c r="CQ227" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR227" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS227" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ227" s="2"/>
+      <c r="CR227" s="2"/>
+      <c r="CS227" s="2"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="n">
@@ -66933,15 +65571,9 @@
       <c r="CP228" s="2" t="n">
         <v>3.705</v>
       </c>
-      <c r="CQ228" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR228" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS228" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ228" s="2"/>
+      <c r="CR228" s="2"/>
+      <c r="CS228" s="2"/>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="n">
@@ -67226,15 +65858,9 @@
       <c r="CP229" s="2" t="n">
         <v>3.718</v>
       </c>
-      <c r="CQ229" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR229" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS229" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ229" s="2"/>
+      <c r="CR229" s="2"/>
+      <c r="CS229" s="2"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="n">
@@ -67519,15 +66145,9 @@
       <c r="CP230" s="2" t="n">
         <v>3.757</v>
       </c>
-      <c r="CQ230" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR230" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS230" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ230" s="2"/>
+      <c r="CR230" s="2"/>
+      <c r="CS230" s="2"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="n">
@@ -67812,15 +66432,9 @@
       <c r="CP231" s="2" t="n">
         <v>3.769</v>
       </c>
-      <c r="CQ231" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR231" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS231" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ231" s="2"/>
+      <c r="CR231" s="2"/>
+      <c r="CS231" s="2"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="n">
@@ -68105,15 +66719,9 @@
       <c r="CP232" s="2" t="n">
         <v>3.881</v>
       </c>
-      <c r="CQ232" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR232" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS232" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ232" s="2"/>
+      <c r="CR232" s="2"/>
+      <c r="CS232" s="2"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="n">
@@ -68398,15 +67006,9 @@
       <c r="CP233" s="2" t="n">
         <v>3.817</v>
       </c>
-      <c r="CQ233" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR233" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS233" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ233" s="2"/>
+      <c r="CR233" s="2"/>
+      <c r="CS233" s="2"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="n">
@@ -68691,15 +67293,9 @@
       <c r="CP234" s="2" t="n">
         <v>3.875</v>
       </c>
-      <c r="CQ234" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR234" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS234" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ234" s="2"/>
+      <c r="CR234" s="2"/>
+      <c r="CS234" s="2"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="n">
@@ -68984,15 +67580,9 @@
       <c r="CP235" s="2" t="n">
         <v>3.889</v>
       </c>
-      <c r="CQ235" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR235" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS235" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ235" s="2"/>
+      <c r="CR235" s="2"/>
+      <c r="CS235" s="2"/>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="n">
@@ -69277,15 +67867,9 @@
       <c r="CP236" s="2" t="n">
         <v>3.906</v>
       </c>
-      <c r="CQ236" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR236" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS236" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ236" s="2"/>
+      <c r="CR236" s="2"/>
+      <c r="CS236" s="2"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="n">
@@ -69570,15 +68154,9 @@
       <c r="CP237" s="2" t="n">
         <v>3.942</v>
       </c>
-      <c r="CQ237" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR237" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS237" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ237" s="2"/>
+      <c r="CR237" s="2"/>
+      <c r="CS237" s="2"/>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="n">
@@ -69863,15 +68441,9 @@
       <c r="CP238" s="2" t="n">
         <v>3.984</v>
       </c>
-      <c r="CQ238" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR238" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS238" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ238" s="2"/>
+      <c r="CR238" s="2"/>
+      <c r="CS238" s="2"/>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="n">
@@ -70156,15 +68728,9 @@
       <c r="CP239" s="2" t="n">
         <v>4.072</v>
       </c>
-      <c r="CQ239" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR239" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS239" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ239" s="2"/>
+      <c r="CR239" s="2"/>
+      <c r="CS239" s="2"/>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="n">
@@ -70449,15 +69015,9 @@
       <c r="CP240" s="2" t="n">
         <v>4.02</v>
       </c>
-      <c r="CQ240" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR240" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS240" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="CQ240" s="2"/>
+      <c r="CR240" s="2"/>
+      <c r="CS240" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>